<commit_message>
added date and decison fields
</commit_message>
<xml_diff>
--- a/Job-tracker/jobs.xlsx
+++ b/Job-tracker/jobs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,24 +436,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Asus</t>
+          <t>uliza</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Not Specified</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>BMW</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ZAR 10000</t>
+          <t>ZAR 7000</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025-01-30</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Pending</t>
         </is>
       </c>
     </row>

</xml_diff>